<commit_message>
Add new excel file template
</commit_message>
<xml_diff>
--- a/moduerp/src/main/webapp/resources/templates/부서직원파일양식.xlsx
+++ b/moduerp/src/main/webapp/resources/templates/부서직원파일양식.xlsx
@@ -2,20 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\moduerp_workspace\moduerp\src\main\webapp\resources\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ict01_27\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0EF8650-1112-498D-8FEC-C7D6D359E8B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4AE0CD-9F84-4D70-8B1A-33625FC71427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="11295" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14460" yWindow="0" windowWidth="24045" windowHeight="15585" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="부서정보" sheetId="1" r:id="rId1"/>
     <sheet name="사원정보" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="departmentNames" comment="부서정보 시트에 동적 범위 설정">OFFSET(부서정보!$A$2, 0, 0, COUNTA(부서정보!$A:$A)-1, 1)</definedName>
+  </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -26,13 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
-  <si>
-    <t>부서코드</t>
-  </si>
-  <si>
-    <t>부서명</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>사원명</t>
   </si>
@@ -42,12 +39,20 @@
   <si>
     <t>사원이메일</t>
   </si>
+  <si>
+    <t>부서명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부서명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -57,6 +62,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -82,7 +95,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -91,57 +104,54 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -235,39 +245,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -319,7 +329,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -430,13 +440,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -445,6 +448,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -509,11 +519,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -521,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" activeCellId="1" sqref="A1:D1 C11"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -534,13 +564,19 @@
     <col min="3" max="1025" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -555,10 +591,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -572,22 +608,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{0EA501AA-94F3-4F84-9AA1-8F1B14D031E3}">
+      <formula1>departmentNames</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix 400 Bad Request by renaming file input and updating DTO binding
- Changed `<input type="file" name="attachment" />` to `<input type="file" name="file" />` to resolve binding issues.
- Updated DTO class to handle file uploads correctly with matching field names.
- Ensured consistency between form field names and DTO properties to prevent data binding errors.
</commit_message>
<xml_diff>
--- a/moduerp/src/main/webapp/resources/templates/부서직원파일양식.xlsx
+++ b/moduerp/src/main/webapp/resources/templates/부서직원파일양식.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ict01_27\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4AE0CD-9F84-4D70-8B1A-33625FC71427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7BA020-271B-457B-AECF-33A6A6E2D71F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14460" yWindow="0" windowWidth="24045" windowHeight="15585" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="부서정보" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>사원명</t>
   </si>
@@ -45,6 +45,10 @@
   </si>
   <si>
     <t>부서명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>직급</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -75,7 +79,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,6 +96,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD1D1D1"/>
         <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -123,29 +133,23 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -551,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -565,18 +569,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="2"/>
+      <c r="B1" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -591,48 +587,86 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
+    <col min="1" max="1" width="18.75" customWidth="1"/>
     <col min="2" max="2" width="16.625" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="14.125" customWidth="1"/>
     <col min="5" max="5" width="21.375" customWidth="1"/>
     <col min="6" max="1025" width="8.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>